<commit_message>
Resultat de la decision final
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lolo_\Documents\GitHub\axrjiopolkj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{7E1C8B4E-4D34-462A-ACAD-B949DC90ECF9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3ACE706D-FCFA-4209-908A-7242BCF7326D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{D26FB3E9-7169-4A2D-8823-43ACBCFA511D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Euclidien</t>
   </si>
@@ -64,13 +64,25 @@
   </si>
   <si>
     <t>dice</t>
+  </si>
+  <si>
+    <t>Corrélation et décalage</t>
+  </si>
+  <si>
+    <t>Corrélation</t>
+  </si>
+  <si>
+    <t>Manhattan et décalage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="175" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,8 +90,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,8 +109,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -101,13 +124,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,152 +475,268 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30609AB0-A111-4F4C-82EB-DD009E279374}">
-  <dimension ref="A2:I7"/>
+  <dimension ref="A2:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="32.42578125" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" customWidth="1"/>
+    <col min="16" max="16" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:16">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="K2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:16">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>0.48</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>0.12</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>0.4</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>0.16</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="6">
         <v>0.48</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>0.44</v>
       </c>
-      <c r="I3">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1">
         <v>0.44</v>
       </c>
+      <c r="K3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0.48</v>
+      </c>
+      <c r="O3" s="7">
+        <v>0.52</v>
+      </c>
+      <c r="P3" s="7">
+        <v>0.44</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:16">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>0.4204</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>0.28889999999999999</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>0.38890000000000002</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>0.245</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="6">
         <v>0.67879999999999996</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>0.59440000000000004</v>
       </c>
-      <c r="I4">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1">
         <v>0.58979999999999999</v>
       </c>
+      <c r="K4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.4204</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0.63227276644352703</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0.67878004829675198</v>
+      </c>
+      <c r="O4" s="7">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="P4" s="7">
+        <v>0.45810000000000001</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:16">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>0.80859999999999999</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>0.4219</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>0.58160000000000001</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>0.65800000000000003</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="6">
         <v>0.79</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>0.7419</v>
       </c>
-      <c r="I5">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1">
         <v>0.75600000000000001</v>
       </c>
+      <c r="K5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0.80859999999999999</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0.73043238586014902</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0.79008896833391395</v>
+      </c>
+      <c r="O5" s="7">
+        <v>0.70240000000000002</v>
+      </c>
+      <c r="P5" s="7">
+        <v>0.64390000000000003</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="6" spans="1:16">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>0.72</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>0.6</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="6">
         <v>0.96</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>0.92</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>0.88</v>
       </c>
-      <c r="I7">
+      <c r="H7" s="1"/>
+      <c r="I7" s="1">
         <v>0.56000000000000005</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0.76</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="O7" s="7">
+        <v>0.73</v>
+      </c>
+      <c r="P7" s="8">
+        <v>0.96</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>